<commit_message>
Save before adding into hosts
</commit_message>
<xml_diff>
--- a/vedv/web/assets/protocols_diuretic.xlsx
+++ b/vedv/web/assets/protocols_diuretic.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="table_for_two_hours-1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="table_for_four_hours-1" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="table_for_two_hours-2" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="table_for_four_hours-2" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="table_for_two_hours-3" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="table_for_four_hours-3" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="table_for_two_hours-4" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="table_for_four_hours-4" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="table_for_two_hours-1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="table_for_four_hours-1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="table_for_two_hours-2" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="table_for_four_hours-2" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="table_for_two_hours-3" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="table_for_four_hours-3" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="table_for_two_hours-4" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="table_for_four_hours-4" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="table_for_two_hours-5" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="table_for_four_hours-5" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -61,18 +63,86 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -391,37 +461,37 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>kk-11</t>
+          <t>34-7</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>kk-5</t>
+          <t>34-8</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>kk-13</t>
+          <t>34-2</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>kk-12</t>
+          <t>34-18</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>kk-3</t>
+          <t>34-4</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>kk-21</t>
+          <t>34-25</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>kk-4</t>
+          <t>34-1</t>
         </is>
       </c>
     </row>
@@ -432,34 +502,34 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="C2" t="n">
-        <v>3.6</v>
+        <v>3.9</v>
       </c>
       <c r="D2" t="n">
-        <v>2.6</v>
+        <v>1.8</v>
       </c>
       <c r="E2" t="n">
-        <v>1.8</v>
+        <v>2.7</v>
       </c>
       <c r="F2" t="n">
-        <v>2.5</v>
+        <v>1.4</v>
       </c>
       <c r="G2" t="n">
-        <v>2.6</v>
+        <v>2.7</v>
       </c>
       <c r="H2" t="n">
-        <v>2.7</v>
+        <v>2.1</v>
       </c>
       <c r="I2" t="n">
-        <v>2.5</v>
+        <v>2.2</v>
       </c>
       <c r="J2" t="n">
-        <v>1.5</v>
+        <v>2.3</v>
       </c>
       <c r="K2" t="n">
-        <v>2.1</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="3">
@@ -469,34 +539,34 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
         <v>3.5</v>
       </c>
       <c r="D3" t="n">
-        <v>2.4</v>
+        <v>1.9</v>
       </c>
       <c r="E3" t="n">
-        <v>2.3</v>
+        <v>1.9</v>
       </c>
       <c r="F3" t="n">
-        <v>2.8</v>
+        <v>1.4</v>
       </c>
       <c r="G3" t="n">
-        <v>2</v>
+        <v>1.3</v>
       </c>
       <c r="H3" t="n">
-        <v>2.4</v>
+        <v>2.1</v>
       </c>
       <c r="I3" t="n">
-        <v>1.9</v>
+        <v>1.3</v>
       </c>
       <c r="J3" t="n">
-        <v>2.2</v>
+        <v>1.4</v>
       </c>
       <c r="K3" t="n">
-        <v>2</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="4">
@@ -506,34 +576,34 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="C4" t="n">
-        <v>4</v>
+        <v>3.9</v>
       </c>
       <c r="D4" t="n">
-        <v>2.5</v>
+        <v>1.7</v>
       </c>
       <c r="E4" t="n">
-        <v>2.1</v>
+        <v>2.8</v>
       </c>
       <c r="F4" t="n">
-        <v>2.2</v>
+        <v>2.3</v>
       </c>
       <c r="G4" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="H4" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="I4" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="K4" t="n">
         <v>1.3</v>
-      </c>
-      <c r="H4" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="I4" t="n">
-        <v>1.7</v>
-      </c>
-      <c r="J4" t="n">
-        <v>2.3</v>
-      </c>
-      <c r="K4" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -543,34 +613,34 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1.1</v>
+        <v>1.6</v>
       </c>
       <c r="C5" t="n">
         <v>3.5</v>
       </c>
       <c r="D5" t="n">
-        <v>2.3</v>
+        <v>2.7</v>
       </c>
       <c r="E5" t="n">
-        <v>2.5</v>
+        <v>2.6</v>
       </c>
       <c r="F5" t="n">
-        <v>2</v>
+        <v>2.7</v>
       </c>
       <c r="G5" t="n">
-        <v>2.2</v>
+        <v>2.4</v>
       </c>
       <c r="H5" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="I5" t="n">
         <v>1.2</v>
       </c>
-      <c r="I5" t="n">
-        <v>1.4</v>
-      </c>
       <c r="J5" t="n">
-        <v>1.1</v>
+        <v>2.8</v>
       </c>
       <c r="K5" t="n">
-        <v>2.8</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="6">
@@ -583,31 +653,31 @@
         <v>1.4</v>
       </c>
       <c r="C6" t="n">
-        <v>3.7</v>
+        <v>3.9</v>
       </c>
       <c r="D6" t="n">
-        <v>1.6</v>
+        <v>2.2</v>
       </c>
       <c r="E6" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="F6" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="G6" t="n">
         <v>2.4</v>
       </c>
-      <c r="F6" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="G6" t="n">
-        <v>1.7</v>
-      </c>
       <c r="H6" t="n">
-        <v>2.3</v>
+        <v>2.8</v>
       </c>
       <c r="I6" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="J6" t="n">
         <v>2.1</v>
       </c>
-      <c r="J6" t="n">
+      <c r="K6" t="n">
         <v>2</v>
-      </c>
-      <c r="K6" t="n">
-        <v>1.5</v>
       </c>
     </row>
     <row r="7">
@@ -617,34 +687,34 @@
         </is>
       </c>
       <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="G7" t="n">
+        <v>2</v>
+      </c>
+      <c r="H7" t="n">
         <v>1.5</v>
       </c>
-      <c r="C7" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="D7" t="n">
-        <v>2.3</v>
-      </c>
-      <c r="E7" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="F7" t="n">
-        <v>2.6</v>
-      </c>
-      <c r="G7" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="H7" t="n">
-        <v>2.2</v>
-      </c>
       <c r="I7" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="K7" t="n">
         <v>1.5</v>
-      </c>
-      <c r="J7" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="K7" t="n">
-        <v>1.2</v>
       </c>
     </row>
     <row r="8">
@@ -654,38 +724,342 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1.8</v>
+        <v>1.7</v>
       </c>
       <c r="C8" t="n">
         <v>3.7</v>
       </c>
       <c r="D8" t="n">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="E8" t="n">
-        <v>1.7</v>
+        <v>2.8</v>
       </c>
       <c r="F8" t="n">
         <v>2.8</v>
       </c>
       <c r="G8" t="n">
-        <v>1.1</v>
+        <v>2.3</v>
       </c>
       <c r="H8" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="J8" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="K8" t="n">
+        <v>1.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Контроль</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Фуросемід</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Гіпотіазид</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>34-11</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>34-13</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>34-23</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>34-10</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>34-9</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>34-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Щур-1</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="F2" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="G2" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="H2" t="n">
+        <v>4</v>
+      </c>
+      <c r="I2" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J2" t="n">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Щур-2</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="C3" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="D3" t="n">
         <v>2</v>
       </c>
+      <c r="E3" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="F3" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="H3" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="I3" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="J3" t="n">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Щур-3</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="C4" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="E4" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="F4" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="H4" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="I4" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="J4" t="n">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Щур-4</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" t="n">
+        <v>6.699999999999999</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="F5" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="G5" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="H5" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="I5" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="J5" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Щур-5</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="C6" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="E6" t="n">
+        <v>4</v>
+      </c>
+      <c r="F6" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="G6" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="H6" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="I6" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J6" t="n">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Щур-6</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="C7" t="n">
+        <v>5.800000000000001</v>
+      </c>
+      <c r="D7" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="F7" t="n">
+        <v>4.199999999999999</v>
+      </c>
+      <c r="G7" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="H7" t="n">
+        <v>3</v>
+      </c>
+      <c r="I7" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="J7" t="n">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Щур-7</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="C8" t="n">
+        <v>5.899999999999999</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="E8" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="F8" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="G8" t="n">
+        <v>3</v>
+      </c>
+      <c r="H8" t="n">
+        <v>4.2</v>
+      </c>
       <c r="I8" t="n">
-        <v>1.8</v>
+        <v>3</v>
       </c>
       <c r="J8" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="K8" t="n">
-        <v>1.9</v>
+        <v>3.7</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -721,37 +1095,37 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>kk-11</t>
+          <t>34-7</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>kk-5</t>
+          <t>34-8</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>kk-13</t>
+          <t>34-2</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>kk-12</t>
+          <t>34-18</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>kk-3</t>
+          <t>34-4</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>kk-21</t>
+          <t>34-25</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>kk-4</t>
+          <t>34-1</t>
         </is>
       </c>
     </row>
@@ -762,34 +1136,34 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1.4</v>
+        <v>1.8</v>
       </c>
       <c r="C2" t="n">
-        <v>5.6</v>
+        <v>5.7</v>
       </c>
       <c r="D2" t="n">
-        <v>3.4</v>
+        <v>2.7</v>
       </c>
       <c r="E2" t="n">
-        <v>3.1</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
-        <v>2.9</v>
+        <v>2.8</v>
       </c>
       <c r="G2" t="n">
-        <v>4.3</v>
+        <v>3.7</v>
       </c>
       <c r="H2" t="n">
-        <v>4.300000000000001</v>
+        <v>3</v>
       </c>
       <c r="I2" t="n">
-        <v>3.9</v>
+        <v>2.8</v>
       </c>
       <c r="J2" t="n">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="K2" t="n">
-        <v>2.7</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="3">
@@ -802,31 +1176,31 @@
         <v>1.7</v>
       </c>
       <c r="C3" t="n">
-        <v>6.1</v>
+        <v>5.3</v>
       </c>
       <c r="D3" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="H3" t="n">
         <v>3.3</v>
       </c>
-      <c r="E3" t="n">
-        <v>4</v>
-      </c>
-      <c r="F3" t="n">
+      <c r="I3" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="J3" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="K3" t="n">
         <v>3.3</v>
-      </c>
-      <c r="G3" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="H3" t="n">
-        <v>2.8</v>
-      </c>
-      <c r="I3" t="n">
-        <v>3.4</v>
-      </c>
-      <c r="J3" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="K3" t="n">
-        <v>2.9</v>
       </c>
     </row>
     <row r="4">
@@ -839,31 +1213,31 @@
         <v>2</v>
       </c>
       <c r="C4" t="n">
-        <v>6.5</v>
+        <v>5.4</v>
       </c>
       <c r="D4" t="n">
-        <v>3.6</v>
+        <v>2.7</v>
       </c>
       <c r="E4" t="n">
+        <v>4</v>
+      </c>
+      <c r="F4" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="G4" t="n">
         <v>2.6</v>
       </c>
-      <c r="F4" t="n">
-        <v>3.3</v>
-      </c>
-      <c r="G4" t="n">
-        <v>3</v>
-      </c>
       <c r="H4" t="n">
-        <v>2.6</v>
+        <v>3.1</v>
       </c>
       <c r="I4" t="n">
-        <v>2.8</v>
+        <v>3.5</v>
       </c>
       <c r="J4" t="n">
-        <v>3.5</v>
+        <v>2.7</v>
       </c>
       <c r="K4" t="n">
-        <v>3.2</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="5">
@@ -873,34 +1247,34 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>2.1</v>
       </c>
       <c r="C5" t="n">
-        <v>5.8</v>
+        <v>5.7</v>
       </c>
       <c r="D5" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="E5" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="F5" t="n">
+        <v>4.300000000000001</v>
+      </c>
+      <c r="G5" t="n">
+        <v>4</v>
+      </c>
+      <c r="H5" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="J5" t="n">
         <v>3.5</v>
       </c>
-      <c r="E5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F5" t="n">
-        <v>3.1</v>
-      </c>
-      <c r="G5" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="H5" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="I5" t="n">
-        <v>2.8</v>
-      </c>
-      <c r="J5" t="n">
-        <v>2.7</v>
-      </c>
       <c r="K5" t="n">
-        <v>3.7</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="6">
@@ -913,31 +1287,31 @@
         <v>2.1</v>
       </c>
       <c r="C6" t="n">
-        <v>6.2</v>
+        <v>6.3</v>
       </c>
       <c r="D6" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="E6" t="n">
+        <v>4</v>
+      </c>
+      <c r="F6" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="G6" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="H6" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="I6" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="J6" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="K6" t="n">
         <v>2.5</v>
-      </c>
-      <c r="E6" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="F6" t="n">
-        <v>2.4</v>
-      </c>
-      <c r="G6" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="H6" t="n">
-        <v>3.3</v>
-      </c>
-      <c r="I6" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="J6" t="n">
-        <v>2.6</v>
-      </c>
-      <c r="K6" t="n">
-        <v>3.1</v>
       </c>
     </row>
     <row r="7">
@@ -947,34 +1321,34 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1.9</v>
+        <v>1.6</v>
       </c>
       <c r="C7" t="n">
-        <v>6.6</v>
+        <v>6</v>
       </c>
       <c r="D7" t="n">
-        <v>3.7</v>
+        <v>3.6</v>
       </c>
       <c r="E7" t="n">
-        <v>1.6</v>
+        <v>2.4</v>
       </c>
       <c r="F7" t="n">
-        <v>3.1</v>
+        <v>1.8</v>
       </c>
       <c r="G7" t="n">
-        <v>3.6</v>
+        <v>3</v>
       </c>
       <c r="H7" t="n">
-        <v>3.9</v>
+        <v>3.2</v>
       </c>
       <c r="I7" t="n">
-        <v>1.9</v>
+        <v>3.4</v>
       </c>
       <c r="J7" t="n">
-        <v>2.7</v>
+        <v>2.9</v>
       </c>
       <c r="K7" t="n">
-        <v>1.9</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="8">
@@ -984,38 +1358,38 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2.2</v>
+        <v>2.6</v>
       </c>
       <c r="C8" t="n">
-        <v>5.5</v>
+        <v>5.9</v>
       </c>
       <c r="D8" t="n">
         <v>2.4</v>
       </c>
       <c r="E8" t="n">
-        <v>3.2</v>
+        <v>4.4</v>
       </c>
       <c r="F8" t="n">
+        <v>4.199999999999999</v>
+      </c>
+      <c r="G8" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="H8" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="I8" t="n">
+        <v>2</v>
+      </c>
+      <c r="J8" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="K8" t="n">
         <v>3.3</v>
       </c>
-      <c r="G8" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="H8" t="n">
-        <v>2.7</v>
-      </c>
-      <c r="I8" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="J8" t="n">
-        <v>2.8</v>
-      </c>
-      <c r="K8" t="n">
-        <v>2.3</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -1051,37 +1425,37 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>kk-20</t>
+          <t>34-30</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>kk-10</t>
+          <t>34-5</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>kk-9</t>
+          <t>34-27</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>kk-8</t>
+          <t>34-28</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>kk-16</t>
+          <t>34-21</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>kk-17</t>
+          <t>34-6</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>kk-1</t>
+          <t>34-22</t>
         </is>
       </c>
     </row>
@@ -1092,34 +1466,34 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>1.1</v>
       </c>
       <c r="C2" t="n">
-        <v>4.3</v>
+        <v>4</v>
       </c>
       <c r="D2" t="n">
-        <v>1.4</v>
+        <v>2</v>
       </c>
       <c r="E2" t="n">
-        <v>1.3</v>
+        <v>2.8</v>
       </c>
       <c r="F2" t="n">
-        <v>2.6</v>
+        <v>1.1</v>
       </c>
       <c r="G2" t="n">
-        <v>1.7</v>
+        <v>2.1</v>
       </c>
       <c r="H2" t="n">
-        <v>1.4</v>
+        <v>2.1</v>
       </c>
       <c r="I2" t="n">
         <v>2.3</v>
       </c>
       <c r="J2" t="n">
-        <v>2.2</v>
+        <v>2.8</v>
       </c>
       <c r="K2" t="n">
-        <v>2.3</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="3">
@@ -1129,34 +1503,34 @@
         </is>
       </c>
       <c r="B3" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="H3" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="I3" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="J3" t="n">
         <v>1.4</v>
       </c>
-      <c r="C3" t="n">
-        <v>3.7</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="E3" t="n">
+      <c r="K3" t="n">
         <v>1.3</v>
-      </c>
-      <c r="F3" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="G3" t="n">
-        <v>2.4</v>
-      </c>
-      <c r="H3" t="n">
-        <v>1.7</v>
-      </c>
-      <c r="I3" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="J3" t="n">
-        <v>2.7</v>
-      </c>
-      <c r="K3" t="n">
-        <v>1.5</v>
       </c>
     </row>
     <row r="4">
@@ -1166,34 +1540,34 @@
         </is>
       </c>
       <c r="B4" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="C4" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="G4" t="n">
         <v>1.1</v>
       </c>
-      <c r="C4" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="D4" t="n">
-        <v>2.3</v>
-      </c>
-      <c r="E4" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="F4" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="I4" t="n">
         <v>2.8</v>
       </c>
-      <c r="H4" t="n">
-        <v>2.8</v>
-      </c>
-      <c r="I4" t="n">
-        <v>1.9</v>
-      </c>
       <c r="J4" t="n">
-        <v>2.6</v>
+        <v>1.3</v>
       </c>
       <c r="K4" t="n">
-        <v>1.7</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="5">
@@ -1203,31 +1577,31 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1.8</v>
+        <v>1.6</v>
       </c>
       <c r="C5" t="n">
-        <v>4</v>
+        <v>4.3</v>
       </c>
       <c r="D5" t="n">
-        <v>2.1</v>
+        <v>2.8</v>
       </c>
       <c r="E5" t="n">
-        <v>1.7</v>
+        <v>2.4</v>
       </c>
       <c r="F5" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="G5" t="n">
         <v>1.3</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="I5" t="n">
+        <v>2</v>
+      </c>
+      <c r="J5" t="n">
         <v>1.4</v>
-      </c>
-      <c r="H5" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="I5" t="n">
-        <v>2.8</v>
-      </c>
-      <c r="J5" t="n">
-        <v>1.3</v>
       </c>
       <c r="K5" t="n">
         <v>2.4</v>
@@ -1240,34 +1614,34 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="C6" t="n">
-        <v>4.1</v>
+        <v>3.5</v>
       </c>
       <c r="D6" t="n">
-        <v>1.3</v>
+        <v>1.9</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>1.1</v>
       </c>
       <c r="F6" t="n">
         <v>1.6</v>
       </c>
       <c r="G6" t="n">
+        <v>2</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="I6" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="J6" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="K6" t="n">
         <v>1.5</v>
-      </c>
-      <c r="H6" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="I6" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="J6" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="K6" t="n">
-        <v>1.6</v>
       </c>
     </row>
     <row r="7">
@@ -1277,7 +1651,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1.6</v>
+        <v>1.1</v>
       </c>
       <c r="C7" t="n">
         <v>4</v>
@@ -1289,22 +1663,22 @@
         <v>2.5</v>
       </c>
       <c r="F7" t="n">
-        <v>1.1</v>
+        <v>2.2</v>
       </c>
       <c r="G7" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="H7" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="I7" t="n">
         <v>1.3</v>
       </c>
-      <c r="H7" t="n">
-        <v>2.3</v>
-      </c>
-      <c r="I7" t="n">
-        <v>1.5</v>
-      </c>
       <c r="J7" t="n">
-        <v>1.2</v>
+        <v>2.2</v>
       </c>
       <c r="K7" t="n">
-        <v>1.7</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="8">
@@ -1314,38 +1688,38 @@
         </is>
       </c>
       <c r="B8" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="C8" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="E8" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="H8" t="n">
+        <v>2</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="J8" t="n">
         <v>1.5</v>
       </c>
-      <c r="C8" t="n">
-        <v>4</v>
-      </c>
-      <c r="D8" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="E8" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="F8" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="G8" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="H8" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="I8" t="n">
-        <v>2</v>
-      </c>
-      <c r="J8" t="n">
-        <v>2</v>
-      </c>
       <c r="K8" t="n">
-        <v>2</v>
+        <v>2.8</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -1381,37 +1755,37 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>kk-20</t>
+          <t>34-30</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>kk-10</t>
+          <t>34-5</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>kk-9</t>
+          <t>34-27</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>kk-8</t>
+          <t>34-28</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>kk-16</t>
+          <t>34-21</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>kk-17</t>
+          <t>34-6</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>kk-1</t>
+          <t>34-22</t>
         </is>
       </c>
     </row>
@@ -1422,34 +1796,34 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1.4</v>
+        <v>1.6</v>
       </c>
       <c r="C2" t="n">
-        <v>6.6</v>
+        <v>6</v>
       </c>
       <c r="D2" t="n">
-        <v>2.7</v>
+        <v>2.9</v>
       </c>
       <c r="E2" t="n">
-        <v>1.8</v>
+        <v>3.5</v>
       </c>
       <c r="F2" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="G2" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="H2" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="I2" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J2" t="n">
         <v>3.9</v>
       </c>
-      <c r="G2" t="n">
-        <v>3.3</v>
-      </c>
-      <c r="H2" t="n">
-        <v>2</v>
-      </c>
-      <c r="I2" t="n">
-        <v>3.7</v>
-      </c>
-      <c r="J2" t="n">
-        <v>2.7</v>
-      </c>
       <c r="K2" t="n">
-        <v>2.8</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="3">
@@ -1459,34 +1833,34 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2.2</v>
+        <v>2.1</v>
       </c>
       <c r="C3" t="n">
-        <v>5.2</v>
+        <v>5.4</v>
       </c>
       <c r="D3" t="n">
-        <v>2.6</v>
+        <v>2.8</v>
       </c>
       <c r="E3" t="n">
-        <v>2.8</v>
+        <v>4.199999999999999</v>
       </c>
       <c r="F3" t="n">
-        <v>2</v>
+        <v>3.2</v>
       </c>
       <c r="G3" t="n">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="H3" t="n">
-        <v>2.4</v>
+        <v>3.9</v>
       </c>
       <c r="I3" t="n">
-        <v>2</v>
+        <v>3.1</v>
       </c>
       <c r="J3" t="n">
-        <v>3.6</v>
+        <v>3.1</v>
       </c>
       <c r="K3" t="n">
-        <v>1.9</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="4">
@@ -1496,34 +1870,34 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.7</v>
+        <v>2</v>
       </c>
       <c r="C4" t="n">
-        <v>6</v>
+        <v>5.6</v>
       </c>
       <c r="D4" t="n">
-        <v>3.7</v>
+        <v>2.5</v>
       </c>
       <c r="E4" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="F4" t="n">
         <v>2.9</v>
       </c>
-      <c r="F4" t="n">
-        <v>3.1</v>
-      </c>
       <c r="G4" t="n">
-        <v>3.3</v>
+        <v>2.5</v>
       </c>
       <c r="H4" t="n">
-        <v>4.1</v>
+        <v>2</v>
       </c>
       <c r="I4" t="n">
-        <v>2.6</v>
+        <v>3.2</v>
       </c>
       <c r="J4" t="n">
-        <v>3.8</v>
+        <v>2.2</v>
       </c>
       <c r="K4" t="n">
-        <v>2.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -1533,34 +1907,34 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2.2</v>
+        <v>2.4</v>
       </c>
       <c r="C5" t="n">
-        <v>5.6</v>
+        <v>6.5</v>
       </c>
       <c r="D5" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="E5" t="n">
         <v>3</v>
       </c>
-      <c r="E5" t="n">
-        <v>3.1</v>
-      </c>
       <c r="F5" t="n">
-        <v>2.8</v>
+        <v>2.1</v>
       </c>
       <c r="G5" t="n">
-        <v>2</v>
+        <v>2.4</v>
       </c>
       <c r="H5" t="n">
-        <v>2.5</v>
+        <v>3.6</v>
       </c>
       <c r="I5" t="n">
-        <v>3.4</v>
+        <v>3.7</v>
       </c>
       <c r="J5" t="n">
-        <v>2.8</v>
+        <v>2.6</v>
       </c>
       <c r="K5" t="n">
-        <v>3.3</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="6">
@@ -1570,34 +1944,34 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1.8</v>
+        <v>2.2</v>
       </c>
       <c r="C6" t="n">
         <v>5.6</v>
       </c>
       <c r="D6" t="n">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="E6" t="n">
-        <v>2.8</v>
+        <v>2.2</v>
       </c>
       <c r="F6" t="n">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="G6" t="n">
-        <v>2.1</v>
+        <v>2.7</v>
       </c>
       <c r="H6" t="n">
-        <v>2.3</v>
+        <v>2.9</v>
       </c>
       <c r="I6" t="n">
-        <v>2.4</v>
+        <v>3.6</v>
       </c>
       <c r="J6" t="n">
-        <v>2.3</v>
+        <v>3.6</v>
       </c>
       <c r="K6" t="n">
-        <v>2.8</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="7">
@@ -1607,34 +1981,34 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="C7" t="n">
-        <v>5.5</v>
+        <v>6.2</v>
       </c>
       <c r="D7" t="n">
-        <v>2.6</v>
+        <v>2.7</v>
       </c>
       <c r="E7" t="n">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="F7" t="n">
-        <v>2</v>
+        <v>3.2</v>
       </c>
       <c r="G7" t="n">
-        <v>1.8</v>
+        <v>3.5</v>
       </c>
       <c r="H7" t="n">
-        <v>3.9</v>
+        <v>3.8</v>
       </c>
       <c r="I7" t="n">
-        <v>2.2</v>
+        <v>1.9</v>
       </c>
       <c r="J7" t="n">
-        <v>2.9</v>
+        <v>3</v>
       </c>
       <c r="K7" t="n">
-        <v>2.1</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="8">
@@ -1644,38 +2018,38 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="C8" t="n">
-        <v>6.6</v>
+        <v>5.6</v>
       </c>
       <c r="D8" t="n">
-        <v>1.9</v>
+        <v>3.6</v>
       </c>
       <c r="E8" t="n">
-        <v>1.9</v>
+        <v>4</v>
       </c>
       <c r="F8" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="G8" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="H8" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="I8" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="J8" t="n">
         <v>3.2</v>
       </c>
-      <c r="G8" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="H8" t="n">
-        <v>3.3</v>
-      </c>
-      <c r="I8" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="J8" t="n">
-        <v>3.5</v>
-      </c>
       <c r="K8" t="n">
-        <v>3.1</v>
+        <v>3.8</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -1711,37 +2085,37 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>kk-6</t>
+          <t>34-26</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>kk-2</t>
+          <t>34-14</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>kk-24</t>
+          <t>34-32</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>kk-7</t>
+          <t>34-24</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>kk-18</t>
+          <t>34-17</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>kk-14</t>
+          <t>34-15</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>kk-15</t>
+          <t>34-16</t>
         </is>
       </c>
     </row>
@@ -1752,10 +2126,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="D2" t="n">
         <v>1.3</v>
@@ -1764,22 +2138,22 @@
         <v>1.4</v>
       </c>
       <c r="F2" t="n">
-        <v>2.6</v>
+        <v>2.4</v>
       </c>
       <c r="G2" t="n">
-        <v>1.1</v>
+        <v>2.1</v>
       </c>
       <c r="H2" t="n">
         <v>2.7</v>
       </c>
       <c r="I2" t="n">
-        <v>2.8</v>
+        <v>2.5</v>
       </c>
       <c r="J2" t="n">
-        <v>1.4</v>
+        <v>1.6</v>
       </c>
       <c r="K2" t="n">
-        <v>1.8</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="3">
@@ -1792,31 +2166,31 @@
         <v>1.3</v>
       </c>
       <c r="C3" t="n">
-        <v>3.7</v>
+        <v>3.6</v>
       </c>
       <c r="D3" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" t="n">
         <v>1.8</v>
       </c>
-      <c r="E3" t="n">
+      <c r="G3" t="n">
         <v>2.8</v>
       </c>
-      <c r="F3" t="n">
+      <c r="H3" t="n">
         <v>1.9</v>
       </c>
-      <c r="G3" t="n">
-        <v>2.3</v>
-      </c>
-      <c r="H3" t="n">
-        <v>2.7</v>
-      </c>
       <c r="I3" t="n">
-        <v>2</v>
+        <v>1.4</v>
       </c>
       <c r="J3" t="n">
-        <v>2.7</v>
+        <v>1.1</v>
       </c>
       <c r="K3" t="n">
-        <v>2.3</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="4">
@@ -1829,31 +2203,31 @@
         <v>1.3</v>
       </c>
       <c r="C4" t="n">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="D4" t="n">
-        <v>1.6</v>
+        <v>1.4</v>
       </c>
       <c r="E4" t="n">
         <v>1.5</v>
       </c>
       <c r="F4" t="n">
-        <v>1.8</v>
+        <v>1.6</v>
       </c>
       <c r="G4" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="I4" t="n">
         <v>2.1</v>
       </c>
-      <c r="H4" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="I4" t="n">
-        <v>1.7</v>
-      </c>
       <c r="J4" t="n">
-        <v>2.5</v>
+        <v>2.3</v>
       </c>
       <c r="K4" t="n">
-        <v>2.3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -1863,34 +2237,34 @@
         </is>
       </c>
       <c r="B5" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="C5" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="F5" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="G5" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="H5" t="n">
+        <v>2</v>
+      </c>
+      <c r="I5" t="n">
         <v>1.4</v>
       </c>
-      <c r="C5" t="n">
-        <v>3.7</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E5" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="F5" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="G5" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="H5" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="I5" t="n">
-        <v>1.3</v>
-      </c>
       <c r="J5" t="n">
-        <v>1.7</v>
+        <v>2.3</v>
       </c>
       <c r="K5" t="n">
-        <v>2.7</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="6">
@@ -1900,34 +2274,34 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1.2</v>
+        <v>1.1</v>
       </c>
       <c r="C6" t="n">
-        <v>3.7</v>
+        <v>4.2</v>
       </c>
       <c r="D6" t="n">
-        <v>2.5</v>
+        <v>2.7</v>
       </c>
       <c r="E6" t="n">
-        <v>2.7</v>
+        <v>1.7</v>
       </c>
       <c r="F6" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="H6" t="n">
         <v>2</v>
       </c>
-      <c r="G6" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="H6" t="n">
+      <c r="I6" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="K6" t="n">
         <v>2.6</v>
-      </c>
-      <c r="I6" t="n">
-        <v>2</v>
-      </c>
-      <c r="J6" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="K6" t="n">
-        <v>1.4</v>
       </c>
     </row>
     <row r="7">
@@ -1940,31 +2314,31 @@
         <v>1.7</v>
       </c>
       <c r="C7" t="n">
-        <v>4.1</v>
+        <v>4.4</v>
       </c>
       <c r="D7" t="n">
-        <v>2.2</v>
+        <v>1.7</v>
       </c>
       <c r="E7" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="G7" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="H7" t="n">
+        <v>2</v>
+      </c>
+      <c r="I7" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="J7" t="n">
         <v>1.3</v>
       </c>
-      <c r="F7" t="n">
-        <v>2.7</v>
-      </c>
-      <c r="G7" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="H7" t="n">
-        <v>2.7</v>
-      </c>
-      <c r="I7" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="J7" t="n">
-        <v>1.1</v>
-      </c>
       <c r="K7" t="n">
-        <v>2.5</v>
+        <v>2.3</v>
       </c>
     </row>
     <row r="8">
@@ -1977,35 +2351,35 @@
         <v>1.3</v>
       </c>
       <c r="C8" t="n">
-        <v>3.9</v>
+        <v>3.8</v>
       </c>
       <c r="D8" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="E8" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="F8" t="n">
         <v>2.8</v>
-      </c>
-      <c r="E8" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="F8" t="n">
-        <v>2.5</v>
       </c>
       <c r="G8" t="n">
         <v>1.8</v>
       </c>
       <c r="H8" t="n">
-        <v>2.5</v>
+        <v>1.9</v>
       </c>
       <c r="I8" t="n">
-        <v>1.4</v>
+        <v>1.9</v>
       </c>
       <c r="J8" t="n">
-        <v>2.6</v>
+        <v>2.7</v>
       </c>
       <c r="K8" t="n">
-        <v>1.2</v>
+        <v>2.2</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -2041,37 +2415,37 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>kk-6</t>
+          <t>34-26</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>kk-2</t>
+          <t>34-14</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>kk-24</t>
+          <t>34-32</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>kk-7</t>
+          <t>34-24</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>kk-18</t>
+          <t>34-17</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>kk-14</t>
+          <t>34-15</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>kk-15</t>
+          <t>34-16</t>
         </is>
       </c>
     </row>
@@ -2082,34 +2456,34 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1.9</v>
+        <v>1.4</v>
       </c>
       <c r="C2" t="n">
-        <v>5.2</v>
+        <v>5.5</v>
       </c>
       <c r="D2" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="F2" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="H2" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="I2" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="J2" t="n">
+        <v>3</v>
+      </c>
+      <c r="K2" t="n">
         <v>2.1</v>
-      </c>
-      <c r="E2" t="n">
-        <v>2.4</v>
-      </c>
-      <c r="F2" t="n">
-        <v>3.9</v>
-      </c>
-      <c r="G2" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="H2" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="I2" t="n">
-        <v>4.1</v>
-      </c>
-      <c r="J2" t="n">
-        <v>2.3</v>
-      </c>
-      <c r="K2" t="n">
-        <v>3.2</v>
       </c>
     </row>
     <row r="3">
@@ -2119,34 +2493,34 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2.2</v>
+        <v>2.1</v>
       </c>
       <c r="C3" t="n">
-        <v>5.2</v>
+        <v>5.5</v>
       </c>
       <c r="D3" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="E3" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="G3" t="n">
+        <v>4</v>
+      </c>
+      <c r="H3" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="I3" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="J3" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="K3" t="n">
         <v>2.6</v>
-      </c>
-      <c r="E3" t="n">
-        <v>4.199999999999999</v>
-      </c>
-      <c r="F3" t="n">
-        <v>3.4</v>
-      </c>
-      <c r="G3" t="n">
-        <v>2.7</v>
-      </c>
-      <c r="H3" t="n">
-        <v>4.1</v>
-      </c>
-      <c r="I3" t="n">
-        <v>3.1</v>
-      </c>
-      <c r="J3" t="n">
-        <v>4.300000000000001</v>
-      </c>
-      <c r="K3" t="n">
-        <v>3.2</v>
       </c>
     </row>
     <row r="4">
@@ -2156,34 +2530,34 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2.2</v>
+        <v>2.1</v>
       </c>
       <c r="C4" t="n">
-        <v>5.800000000000001</v>
+        <v>5.5</v>
       </c>
       <c r="D4" t="n">
-        <v>2.4</v>
+        <v>2.8</v>
       </c>
       <c r="E4" t="n">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="F4" t="n">
         <v>2.4</v>
       </c>
       <c r="G4" t="n">
-        <v>2.6</v>
+        <v>3.2</v>
       </c>
       <c r="H4" t="n">
-        <v>3</v>
+        <v>1.7</v>
       </c>
       <c r="I4" t="n">
-        <v>3.3</v>
+        <v>3.6</v>
       </c>
       <c r="J4" t="n">
-        <v>3.9</v>
+        <v>2.9</v>
       </c>
       <c r="K4" t="n">
-        <v>2.8</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="5">
@@ -2193,34 +2567,34 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2.2</v>
+        <v>2.5</v>
       </c>
       <c r="C5" t="n">
-        <v>5.4</v>
+        <v>6.4</v>
       </c>
       <c r="D5" t="n">
-        <v>3.3</v>
+        <v>2.9</v>
       </c>
       <c r="E5" t="n">
-        <v>2.6</v>
+        <v>2.7</v>
       </c>
       <c r="F5" t="n">
-        <v>2.1</v>
+        <v>3</v>
       </c>
       <c r="G5" t="n">
-        <v>2.2</v>
+        <v>3</v>
       </c>
       <c r="H5" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="I5" t="n">
         <v>2.6</v>
       </c>
       <c r="J5" t="n">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="K5" t="n">
-        <v>3.5</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="6">
@@ -2230,34 +2604,34 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="C6" t="n">
-        <v>5.6</v>
+        <v>6.800000000000001</v>
       </c>
       <c r="D6" t="n">
-        <v>3.9</v>
+        <v>4</v>
       </c>
       <c r="E6" t="n">
-        <v>4.300000000000001</v>
+        <v>2.2</v>
       </c>
       <c r="F6" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="G6" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="H6" t="n">
         <v>3.3</v>
       </c>
-      <c r="G6" t="n">
-        <v>3.9</v>
-      </c>
-      <c r="H6" t="n">
-        <v>4</v>
-      </c>
       <c r="I6" t="n">
-        <v>2.8</v>
+        <v>3</v>
       </c>
       <c r="J6" t="n">
-        <v>2.4</v>
+        <v>1.9</v>
       </c>
       <c r="K6" t="n">
-        <v>2.5</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="7">
@@ -2267,34 +2641,34 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2.4</v>
+        <v>2.3</v>
       </c>
       <c r="C7" t="n">
-        <v>6.1</v>
+        <v>6.7</v>
       </c>
       <c r="D7" t="n">
         <v>3.1</v>
       </c>
       <c r="E7" t="n">
-        <v>2.8</v>
+        <v>1.8</v>
       </c>
       <c r="F7" t="n">
-        <v>4.4</v>
+        <v>2.2</v>
       </c>
       <c r="G7" t="n">
-        <v>2</v>
+        <v>3.1</v>
       </c>
       <c r="H7" t="n">
-        <v>3.9</v>
+        <v>2.9</v>
       </c>
       <c r="I7" t="n">
-        <v>2.8</v>
+        <v>2.9</v>
       </c>
       <c r="J7" t="n">
-        <v>2.4</v>
+        <v>2.7</v>
       </c>
       <c r="K7" t="n">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="8">
@@ -2304,38 +2678,38 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="C8" t="n">
-        <v>5.7</v>
+        <v>5.5</v>
       </c>
       <c r="D8" t="n">
-        <v>3.7</v>
+        <v>3.1</v>
       </c>
       <c r="E8" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="F8" t="n">
+        <v>4.199999999999999</v>
+      </c>
+      <c r="G8" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="H8" t="n">
         <v>3.2</v>
       </c>
-      <c r="F8" t="n">
+      <c r="I8" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="J8" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="K8" t="n">
         <v>3.2</v>
       </c>
-      <c r="G8" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="H8" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="I8" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="J8" t="n">
-        <v>4.3</v>
-      </c>
-      <c r="K8" t="n">
-        <v>2</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -2345,7 +2719,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2371,22 +2745,37 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>kk-23</t>
+          <t>34-3</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>kk-22</t>
+          <t>34-12</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>kk-19</t>
+          <t>34-33</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>kk-25</t>
+          <t>34-31</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>34-29</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>34-19</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>34-34</t>
         </is>
       </c>
     </row>
@@ -2400,22 +2789,31 @@
         <v>1.7</v>
       </c>
       <c r="C2" t="n">
-        <v>4.4</v>
+        <v>3.6</v>
       </c>
       <c r="D2" t="n">
-        <v>2.6</v>
+        <v>2.4</v>
       </c>
       <c r="E2" t="n">
-        <v>1.4</v>
+        <v>1.6</v>
       </c>
       <c r="F2" t="n">
-        <v>2.4</v>
+        <v>2.2</v>
       </c>
       <c r="G2" t="n">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="H2" t="n">
-        <v>1.4</v>
+        <v>1.1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="J2" t="n">
+        <v>2</v>
+      </c>
+      <c r="K2" t="n">
+        <v>2.2</v>
       </c>
     </row>
     <row r="3">
@@ -2425,25 +2823,34 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
       <c r="C3" t="n">
-        <v>4</v>
+        <v>4.3</v>
       </c>
       <c r="D3" t="n">
-        <v>1.4</v>
+        <v>2</v>
       </c>
       <c r="E3" t="n">
-        <v>1.3</v>
+        <v>2.5</v>
       </c>
       <c r="F3" t="n">
-        <v>1.7</v>
+        <v>2.5</v>
       </c>
       <c r="G3" t="n">
-        <v>1.1</v>
+        <v>1.9</v>
       </c>
       <c r="H3" t="n">
-        <v>2</v>
+        <v>2.5</v>
+      </c>
+      <c r="I3" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="J3" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="K3" t="n">
+        <v>2.6</v>
       </c>
     </row>
     <row r="4">
@@ -2453,25 +2860,34 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.1</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>4.1</v>
+        <v>3.7</v>
       </c>
       <c r="D4" t="n">
-        <v>1.3</v>
+        <v>2.3</v>
       </c>
       <c r="E4" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="G4" t="n">
         <v>2.2</v>
       </c>
-      <c r="F4" t="n">
-        <v>2.4</v>
-      </c>
-      <c r="G4" t="n">
-        <v>2.5</v>
-      </c>
       <c r="H4" t="n">
-        <v>1.4</v>
+        <v>1.7</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="J4" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="K4" t="n">
+        <v>2.7</v>
       </c>
     </row>
     <row r="5">
@@ -2481,25 +2897,34 @@
         </is>
       </c>
       <c r="B5" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="H5" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="J5" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="K5" t="n">
         <v>1.7</v>
-      </c>
-      <c r="C5" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="D5" t="n">
-        <v>2.4</v>
-      </c>
-      <c r="E5" t="n">
-        <v>2.7</v>
-      </c>
-      <c r="F5" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="G5" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="H5" t="n">
-        <v>1.8</v>
       </c>
     </row>
     <row r="6">
@@ -2509,25 +2934,34 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="C6" t="n">
-        <v>4.3</v>
+        <v>3.9</v>
       </c>
       <c r="D6" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="F6" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="G6" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I6" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="J6" t="n">
         <v>2.4</v>
       </c>
-      <c r="E6" t="n">
-        <v>2.8</v>
-      </c>
-      <c r="F6" t="n">
-        <v>2.4</v>
-      </c>
-      <c r="G6" t="n">
-        <v>2.4</v>
-      </c>
-      <c r="H6" t="n">
-        <v>2.6</v>
+      <c r="K6" t="n">
+        <v>2.3</v>
       </c>
     </row>
     <row r="7">
@@ -2537,25 +2971,34 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1.6</v>
+        <v>1.4</v>
       </c>
       <c r="C7" t="n">
-        <v>3.7</v>
+        <v>4.2</v>
       </c>
       <c r="D7" t="n">
-        <v>1.7</v>
+        <v>1.3</v>
       </c>
       <c r="E7" t="n">
         <v>1.9</v>
       </c>
       <c r="F7" t="n">
-        <v>2.3</v>
+        <v>1.3</v>
       </c>
       <c r="G7" t="n">
-        <v>1.4</v>
+        <v>1.9</v>
       </c>
       <c r="H7" t="n">
-        <v>2.4</v>
+        <v>1.6</v>
+      </c>
+      <c r="I7" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="K7" t="n">
+        <v>1.9</v>
       </c>
     </row>
     <row r="8">
@@ -2568,26 +3011,35 @@
         <v>1.8</v>
       </c>
       <c r="C8" t="n">
-        <v>3.5</v>
+        <v>3.8</v>
       </c>
       <c r="D8" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="E8" t="n">
         <v>2.6</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>1.3</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="H8" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="I8" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="J8" t="n">
+        <v>2</v>
+      </c>
+      <c r="K8" t="n">
         <v>2.8</v>
       </c>
-      <c r="G8" t="n">
-        <v>2.6</v>
-      </c>
-      <c r="H8" t="n">
-        <v>2.4</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -2597,7 +3049,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2623,22 +3075,37 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>kk-23</t>
+          <t>34-3</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>kk-22</t>
+          <t>34-12</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>kk-19</t>
+          <t>34-33</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>kk-25</t>
+          <t>34-31</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>34-29</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>34-19</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>34-34</t>
         </is>
       </c>
     </row>
@@ -2649,25 +3116,34 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2.4</v>
+        <v>2.6</v>
       </c>
       <c r="C2" t="n">
-        <v>6.2</v>
+        <v>5.9</v>
       </c>
       <c r="D2" t="n">
-        <v>3.7</v>
+        <v>3.2</v>
       </c>
       <c r="E2" t="n">
-        <v>2.2</v>
+        <v>2.1</v>
       </c>
       <c r="F2" t="n">
-        <v>3.2</v>
+        <v>2.8</v>
       </c>
       <c r="G2" t="n">
-        <v>2.3</v>
+        <v>1.8</v>
       </c>
       <c r="H2" t="n">
-        <v>2.3</v>
+        <v>1.9</v>
+      </c>
+      <c r="I2" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="J2" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="K2" t="n">
+        <v>3.6</v>
       </c>
     </row>
     <row r="3">
@@ -2677,24 +3153,33 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.9</v>
+        <v>2.2</v>
       </c>
       <c r="C3" t="n">
-        <v>5.7</v>
+        <v>6.5</v>
       </c>
       <c r="D3" t="n">
-        <v>2.3</v>
+        <v>3.2</v>
       </c>
       <c r="E3" t="n">
-        <v>2.3</v>
+        <v>3.6</v>
       </c>
       <c r="F3" t="n">
         <v>3</v>
       </c>
       <c r="G3" t="n">
-        <v>2.4</v>
+        <v>2.5</v>
       </c>
       <c r="H3" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="I3" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J3" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="K3" t="n">
         <v>3.4</v>
       </c>
     </row>
@@ -2708,22 +3193,31 @@
         <v>1.6</v>
       </c>
       <c r="C4" t="n">
-        <v>6.3</v>
+        <v>6.300000000000001</v>
       </c>
       <c r="D4" t="n">
-        <v>2.7</v>
+        <v>3.7</v>
       </c>
       <c r="E4" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="G4" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="H4" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="I4" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="J4" t="n">
+        <v>4.300000000000001</v>
+      </c>
+      <c r="K4" t="n">
         <v>3.5</v>
-      </c>
-      <c r="F4" t="n">
-        <v>3</v>
-      </c>
-      <c r="G4" t="n">
-        <v>3.4</v>
-      </c>
-      <c r="H4" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -2733,25 +3227,34 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2.3</v>
+        <v>1.6</v>
       </c>
       <c r="C5" t="n">
-        <v>6.4</v>
+        <v>5.7</v>
       </c>
       <c r="D5" t="n">
-        <v>3.5</v>
+        <v>2.9</v>
       </c>
       <c r="E5" t="n">
-        <v>3.3</v>
+        <v>3</v>
       </c>
       <c r="F5" t="n">
+        <v>2</v>
+      </c>
+      <c r="G5" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="H5" t="n">
         <v>3.7</v>
       </c>
-      <c r="G5" t="n">
-        <v>3.1</v>
-      </c>
-      <c r="H5" t="n">
-        <v>2.8</v>
+      <c r="I5" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="J5" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="K5" t="n">
+        <v>3.4</v>
       </c>
     </row>
     <row r="6">
@@ -2761,25 +3264,34 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1.4</v>
+        <v>1.7</v>
       </c>
       <c r="C6" t="n">
-        <v>5.8</v>
+        <v>6</v>
       </c>
       <c r="D6" t="n">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="E6" t="n">
-        <v>4.4</v>
+        <v>2</v>
       </c>
       <c r="F6" t="n">
-        <v>3.9</v>
+        <v>3.5</v>
       </c>
       <c r="G6" t="n">
-        <v>2.8</v>
+        <v>3.6</v>
       </c>
       <c r="H6" t="n">
-        <v>3.4</v>
+        <v>2.1</v>
+      </c>
+      <c r="I6" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="J6" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="K6" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="7">
@@ -2792,22 +3304,31 @@
         <v>2.1</v>
       </c>
       <c r="C7" t="n">
-        <v>5.7</v>
+        <v>6</v>
       </c>
       <c r="D7" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3</v>
+      </c>
+      <c r="F7" t="n">
+        <v>3</v>
+      </c>
+      <c r="G7" t="n">
         <v>3.1</v>
       </c>
-      <c r="E7" t="n">
-        <v>2.3</v>
-      </c>
-      <c r="F7" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="G7" t="n">
-        <v>2.6</v>
-      </c>
       <c r="H7" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="I7" t="n">
         <v>4.1</v>
+      </c>
+      <c r="J7" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="K7" t="n">
+        <v>2.8</v>
       </c>
     </row>
     <row r="8">
@@ -2817,28 +3338,341 @@
         </is>
       </c>
       <c r="B8" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="C8" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="D8" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="E8" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="G8" t="n">
+        <v>2</v>
+      </c>
+      <c r="H8" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="I8" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="J8" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="K8" t="n">
+        <v>4.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Контроль</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Фуросемід</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Гіпотіазид</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>34-11</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>34-13</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>34-23</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>34-10</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>34-9</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>34-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Щур-1</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="C2" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="G2" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="H2" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="I2" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="J2" t="n">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Щур-2</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Щур-3</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="H4" t="n">
         <v>2.6</v>
       </c>
+      <c r="I4" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Щур-4</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="G5" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="I5" t="n">
+        <v>2</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Щур-5</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="C6" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="H6" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Щур-6</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="C7" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="E7" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="F7" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="J7" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Щур-7</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1.6</v>
+      </c>
       <c r="C8" t="n">
-        <v>5.1</v>
+        <v>4.1</v>
       </c>
       <c r="D8" t="n">
-        <v>3.8</v>
+        <v>1.3</v>
       </c>
       <c r="E8" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="H8" t="n">
         <v>2.6</v>
       </c>
-      <c r="F8" t="n">
-        <v>3.9</v>
-      </c>
-      <c r="G8" t="n">
-        <v>4.3</v>
-      </c>
-      <c r="H8" t="n">
-        <v>3.7</v>
+      <c r="I8" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="J8" t="n">
+        <v>2.8</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>